<commit_message>
Cloud Computer ajustes 20Jun2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 CLOUD computer 01Maio2023 yduqs.xlsx
+++ b/03 Assessments/notas AV1 CLOUD computer 01Maio2023 yduqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\23 WydenArea1ComputacaoNuvemWebServicesLinux\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BBFC38-06A3-45DD-B332-CCED3451B052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B551F0C-F73B-4942-BB68-61C1E074B1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Equipe</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>***</t>
+  </si>
+  <si>
+    <t>Desistiu</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,14 +363,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -686,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,22 +753,22 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="10">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10">
-        <v>2</v>
-      </c>
-      <c r="J5" s="9"/>
+      <c r="D5" s="14"/>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="8"/>
       <c r="K5">
         <v>0</v>
       </c>
@@ -782,22 +783,22 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="10">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10">
-        <v>2</v>
-      </c>
-      <c r="J6" s="11"/>
+      <c r="D6" s="14"/>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="9"/>
       <c r="K6">
         <v>0</v>
       </c>
@@ -809,35 +810,31 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8">
-        <v>2</v>
-      </c>
-      <c r="J8" s="9"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="8"/>
       <c r="K8" s="4">
         <v>1</v>
       </c>
@@ -852,37 +849,33 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10">
-        <v>2</v>
-      </c>
-      <c r="J10" s="9"/>
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="8"/>
       <c r="K10">
         <v>0.5</v>
       </c>
@@ -897,22 +890,21 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11"/>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9"/>
       <c r="M11" s="4">
         <v>7.5</v>
       </c>
@@ -921,58 +913,53 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C12" s="10" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10">
-        <v>0</v>
-      </c>
-      <c r="J12" s="11"/>
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9"/>
       <c r="M12" s="4">
         <v>7.5</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
+      <c r="D13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="9">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10">
-        <v>0</v>
-      </c>
-      <c r="J14" s="9"/>
+      <c r="D14" s="8">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8"/>
       <c r="K14">
         <v>2</v>
       </c>
@@ -987,35 +974,31 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
+      <c r="D15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="8">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8">
-        <v>2</v>
-      </c>
-      <c r="J16" s="9"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="4">
+        <v>2</v>
+      </c>
+      <c r="J16" s="8"/>
       <c r="K16">
         <v>2</v>
       </c>
@@ -1030,22 +1013,21 @@
       </c>
     </row>
     <row r="17" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C17" s="10" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="11">
-        <v>2</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="8">
-        <v>2</v>
-      </c>
-      <c r="J17" s="11"/>
+      <c r="D17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="9"/>
       <c r="K17">
         <v>2</v>
       </c>
@@ -1057,37 +1039,33 @@
       </c>
     </row>
     <row r="18" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9">
-        <v>2</v>
-      </c>
-      <c r="E19" s="10">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="8">
-        <v>1</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8">
-        <v>2</v>
-      </c>
-      <c r="J19" s="9"/>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="8"/>
       <c r="K19">
         <v>1.5</v>
       </c>
@@ -1099,37 +1077,33 @@
       </c>
     </row>
     <row r="20" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>7</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="9">
-        <v>2</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>0.5</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10">
-        <v>1</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10">
-        <v>0</v>
-      </c>
-      <c r="J21" s="9"/>
+      <c r="F21" s="8"/>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8"/>
       <c r="K21">
         <v>2</v>
       </c>
@@ -1144,22 +1118,22 @@
       </c>
     </row>
     <row r="22" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C22" s="10" t="s">
+      <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="10">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10">
-        <v>1</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-      <c r="J22" s="11"/>
+      <c r="D22" s="14"/>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9"/>
       <c r="K22">
         <v>2</v>
       </c>
@@ -1168,37 +1142,33 @@
       </c>
     </row>
     <row r="23" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="J23" s="9"/>
     </row>
     <row r="24" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>8</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="9">
-        <v>2</v>
-      </c>
-      <c r="E24" s="10">
-        <v>1</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10">
-        <v>1</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10">
-        <v>0</v>
-      </c>
-      <c r="J24" s="9"/>
+      <c r="D24" s="8">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="8"/>
       <c r="K24">
         <v>2</v>
       </c>
@@ -1216,20 +1186,18 @@
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="13">
-        <v>2</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="10">
+      <c r="D25" s="11">
+        <v>2</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25">
         <v>0.5</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="13"/>
+      <c r="H25" s="11"/>
+      <c r="J25" s="11"/>
       <c r="M25">
         <v>8</v>
       </c>
@@ -1238,37 +1206,33 @@
       </c>
     </row>
     <row r="26" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="11"/>
+      <c r="D26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>9</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="13">
-        <v>2</v>
-      </c>
-      <c r="E27" s="10">
-        <v>1</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="10">
-        <v>1</v>
-      </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="10">
-        <v>0</v>
-      </c>
-      <c r="J27" s="13"/>
+      <c r="D27" s="11">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" s="11"/>
       <c r="K27">
         <v>0</v>
       </c>
@@ -1283,37 +1247,33 @@
       </c>
     </row>
     <row r="28" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="11"/>
+      <c r="D28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>10</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="11">
-        <v>2</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10">
-        <v>1</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="10">
-        <v>2</v>
-      </c>
-      <c r="J29" s="11"/>
+      <c r="D29" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" s="9"/>
       <c r="K29">
         <v>1</v>
       </c>
@@ -1328,24 +1288,24 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="11">
-        <v>2</v>
-      </c>
-      <c r="E30" s="10">
-        <v>1</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10">
-        <v>1</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="10">
-        <v>2</v>
-      </c>
-      <c r="J30" s="11"/>
+      <c r="D30" s="9">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30" s="9"/>
       <c r="K30">
         <v>1</v>
       </c>
@@ -1360,37 +1320,33 @@
       </c>
     </row>
     <row r="31" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="11"/>
+      <c r="D31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>11</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="11">
-        <v>2</v>
-      </c>
-      <c r="E32" s="10">
-        <v>0</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="10">
-        <v>1</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="10">
-        <v>2</v>
-      </c>
-      <c r="J32" s="11"/>
+      <c r="D32" s="9">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="9"/>
       <c r="K32">
         <v>2</v>
       </c>
@@ -1405,61 +1361,57 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C33" s="10" t="s">
+      <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="11">
-        <v>2</v>
-      </c>
-      <c r="E33" s="10">
-        <v>0</v>
-      </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="10">
-        <v>1</v>
-      </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="10">
-        <v>2</v>
-      </c>
-      <c r="J33" s="11"/>
+      <c r="D33" s="9">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33" s="9"/>
       <c r="M33">
         <v>7.5</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="11"/>
+      <c r="D34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="J34" s="9"/>
     </row>
     <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35">
         <v>12</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="15">
-        <v>2</v>
-      </c>
-      <c r="E35" s="10">
-        <v>1</v>
-      </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="10">
-        <v>1</v>
-      </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="10">
-        <v>0</v>
-      </c>
-      <c r="J35" s="15"/>
+      <c r="D35" s="13">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="13"/>
       <c r="K35">
         <v>2</v>
       </c>
@@ -1474,14 +1426,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="11"/>
+      <c r="D36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="J36" s="9"/>
       <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -1489,22 +1437,22 @@
       <c r="B37">
         <v>13</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="10">
-        <v>1</v>
-      </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="10">
-        <v>1</v>
-      </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="10">
-        <v>2</v>
-      </c>
-      <c r="J37" s="11"/>
+      <c r="D37" s="14"/>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" s="9"/>
       <c r="K37" s="1">
         <v>0</v>
       </c>
@@ -1519,14 +1467,10 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="11"/>
+      <c r="D38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -1535,24 +1479,24 @@
       <c r="B39">
         <v>14</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="15">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10">
-        <v>0</v>
-      </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="10">
-        <v>1</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="10">
-        <v>0</v>
-      </c>
-      <c r="J39" s="11"/>
+      <c r="D39" s="13">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" s="9"/>
       <c r="K39">
         <v>1</v>
       </c>
@@ -1573,8 +1517,29 @@
       <c r="C41" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="15">
-        <v>2</v>
+      <c r="D41" s="13">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="N41" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>